<commit_message>
full orders excel download support added
</commit_message>
<xml_diff>
--- a/backend/cmd/заказы.xlsx
+++ b/backend/cmd/заказы.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ID заказа</t>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>Количество</t>
-  </si>
-  <si>
-    <t>[</t>
   </si>
 </sst>
 </file>
@@ -370,8 +367,105 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>555</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>32313131</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1000</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>44</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
+      </c>
+      <c r="D7">
         <v>5</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
position in sellers display added
</commit_message>
<xml_diff>
--- a/backend/cmd/заказы.xlsx
+++ b/backend/cmd/заказы.xlsx
@@ -468,6 +468,57 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>1464</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>12221</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added position display in adminpanel
</commit_message>
<xml_diff>
--- a/backend/cmd/заказы.xlsx
+++ b/backend/cmd/заказы.xlsx
@@ -368,155 +368,53 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>2200</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5998</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="E3">
         <v>2</v>
-      </c>
-      <c r="C3">
-        <v>555</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
+        <v>31</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
+        <v>10000</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>32313131</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
       <c r="E4">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1000</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>24</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>44</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>25</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>400</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>26</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>27</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>1464</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>12221</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added date_created in excel file
</commit_message>
<xml_diff>
--- a/backend/cmd/заказы.xlsx
+++ b/backend/cmd/заказы.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ID заказа</t>
   </si>
@@ -30,6 +30,18 @@
   </si>
   <si>
     <t>Количество</t>
+  </si>
+  <si>
+    <t>Дата создания</t>
+  </si>
+  <si>
+    <t>2024 01 08 04:43:42</t>
+  </si>
+  <si>
+    <t>2024 01 08 04:44:01</t>
+  </si>
+  <si>
+    <t>2024 01 08 16:54:34</t>
   </si>
 </sst>
 </file>
@@ -365,6 +377,9 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -382,6 +397,9 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -399,6 +417,9 @@
       <c r="E3">
         <v>2</v>
       </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -416,6 +437,9 @@
       <c r="E4">
         <v>10</v>
       </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>